<commit_message>
Funcao listar produtos adicionada
</commit_message>
<xml_diff>
--- a/src/main/resources/temp/chambers.xlsx
+++ b/src/main/resources/temp/chambers.xlsx
@@ -468,7 +468,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A826" workbookViewId="0">
-      <selection activeCell="B865" sqref="B865"/>
+    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -846,7 +846,7 @@
         <v>4023</v>
       </c>
       <c r="B23">
-        <v>-89</v>
+        <v>89</v>
       </c>
       <c r="C23">
         <v>12</v>

</xml_diff>

<commit_message>
versao estavel. em testes
</commit_message>
<xml_diff>
--- a/src/main/resources/temp/chambers.xlsx
+++ b/src/main/resources/temp/chambers.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8064" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7636" uniqueCount="35">
   <si>
     <t>CAM03</t>
   </si>
@@ -130,8 +130,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -159,9 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -478,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H2016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A1379" workbookViewId="0">
+      <selection activeCell="H1409" sqref="H1409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -26664,7 +26674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1249" spans="1:8">
+    <row r="1249" spans="1:7">
       <c r="D1249" t="s">
         <v>0</v>
       </c>
@@ -26678,7 +26688,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1250" spans="1:8">
+    <row r="1250" spans="1:7">
       <c r="D1250" t="s">
         <v>0</v>
       </c>
@@ -26692,7 +26702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1251" spans="1:8">
+    <row r="1251" spans="1:7">
       <c r="D1251" t="s">
         <v>0</v>
       </c>
@@ -26706,7 +26716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1252" spans="1:8">
+    <row r="1252" spans="1:7">
       <c r="D1252" t="s">
         <v>0</v>
       </c>
@@ -26720,7 +26730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1253" spans="1:8">
+    <row r="1253" spans="1:7">
       <c r="D1253" t="s">
         <v>0</v>
       </c>
@@ -26734,7 +26744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1254" spans="1:8">
+    <row r="1254" spans="1:7">
       <c r="D1254" t="s">
         <v>0</v>
       </c>
@@ -26748,7 +26758,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1255" spans="1:8">
+    <row r="1255" spans="1:7">
       <c r="D1255" t="s">
         <v>0</v>
       </c>
@@ -26762,7 +26772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1256" spans="1:8">
+    <row r="1256" spans="1:7">
       <c r="D1256" t="s">
         <v>0</v>
       </c>
@@ -26776,7 +26786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1257" spans="1:8">
+    <row r="1257" spans="1:7">
       <c r="D1257" t="s">
         <v>0</v>
       </c>
@@ -26790,7 +26800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1258" spans="1:8">
+    <row r="1258" spans="1:7">
       <c r="D1258" t="s">
         <v>0</v>
       </c>
@@ -26804,7 +26814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1259" spans="1:8">
+    <row r="1259" spans="1:7">
       <c r="D1259" t="s">
         <v>0</v>
       </c>
@@ -26818,7 +26828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1260" spans="1:8">
+    <row r="1260" spans="1:7">
       <c r="D1260" t="s">
         <v>0</v>
       </c>
@@ -26832,539 +26842,65 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1261" spans="1:8">
-      <c r="A1261" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1261">
-        <v>81</v>
-      </c>
-      <c r="C1261">
-        <v>33</v>
-      </c>
-      <c r="D1261" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1261" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1261" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1261" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1261">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1262" spans="1:8">
-      <c r="A1262" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1262">
-        <v>80</v>
-      </c>
-      <c r="C1262">
-        <v>56</v>
-      </c>
-      <c r="D1262" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1262" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1262" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1262" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1262">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1263" spans="1:8">
-      <c r="A1263" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1263">
-        <v>80</v>
-      </c>
-      <c r="C1263">
-        <v>56</v>
-      </c>
-      <c r="D1263" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1263" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1263" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1263" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1263">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1264" spans="1:8">
-      <c r="D1264" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1264" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1264" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1264" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1265" spans="1:8">
-      <c r="A1265" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1265">
-        <v>77</v>
-      </c>
-      <c r="C1265">
-        <v>56</v>
-      </c>
-      <c r="D1265" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1265" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1265" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1265" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1265">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1266" spans="1:8">
-      <c r="A1266" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1266">
-        <v>74</v>
-      </c>
-      <c r="C1266">
-        <v>56</v>
-      </c>
-      <c r="D1266" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1266" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1266" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1266">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1267" spans="1:8">
-      <c r="A1267" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1267">
-        <v>77</v>
-      </c>
-      <c r="C1267">
-        <v>56</v>
-      </c>
-      <c r="D1267" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1267" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1267" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1267" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1267">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1268" spans="1:8">
-      <c r="A1268" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1268">
-        <v>80</v>
-      </c>
-      <c r="C1268">
-        <v>56</v>
-      </c>
-      <c r="D1268" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1268" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1268" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1268" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1268">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1269" spans="1:8">
-      <c r="A1269" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1269">
-        <v>74</v>
-      </c>
-      <c r="C1269">
-        <v>56</v>
-      </c>
-      <c r="D1269" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1269" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1269" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1269" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1269">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1270" spans="1:8">
-      <c r="A1270" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1270">
-        <v>81</v>
-      </c>
-      <c r="C1270">
-        <v>56</v>
-      </c>
-      <c r="D1270" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1270" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1270" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1270" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1270">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1271" spans="1:8">
-      <c r="A1271" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1271">
-        <v>77</v>
-      </c>
-      <c r="C1271">
-        <v>56</v>
-      </c>
-      <c r="D1271" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1271" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1271" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1271" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1271">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1272" spans="1:8">
-      <c r="A1272" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1272">
-        <v>80</v>
-      </c>
-      <c r="C1272">
-        <v>56</v>
-      </c>
-      <c r="D1272" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1272" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1272" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1272" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1272">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1273" spans="1:8">
-      <c r="A1273" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1273">
-        <v>81</v>
-      </c>
-      <c r="C1273">
-        <v>56</v>
-      </c>
-      <c r="D1273" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1273" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1273" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1273" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1273">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1274" spans="1:8">
-      <c r="A1274" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1274">
-        <v>77</v>
-      </c>
-      <c r="C1274">
-        <v>56</v>
-      </c>
-      <c r="D1274" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1274" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1274" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1274" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1274">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1275" spans="1:8">
-      <c r="A1275" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1275">
-        <v>77</v>
-      </c>
-      <c r="C1275">
-        <v>56</v>
-      </c>
-      <c r="D1275" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1275" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1275" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1275" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1275">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1276" spans="1:8">
-      <c r="A1276" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1276">
-        <v>81</v>
-      </c>
-      <c r="C1276">
-        <v>56</v>
-      </c>
-      <c r="D1276" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1276" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1276" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1276" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1276">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1277" spans="1:8">
-      <c r="A1277" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1277">
-        <v>81</v>
-      </c>
-      <c r="C1277">
-        <v>56</v>
-      </c>
-      <c r="D1277" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1277" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1277" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1277" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1277">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1278" spans="1:8">
-      <c r="A1278" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1278">
-        <v>80</v>
-      </c>
-      <c r="C1278">
-        <v>56</v>
-      </c>
-      <c r="D1278" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1278" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1278" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1278" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1278">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1279" spans="1:8">
-      <c r="A1279" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1279">
-        <v>82</v>
-      </c>
-      <c r="C1279">
-        <v>56</v>
-      </c>
-      <c r="D1279" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1279" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1279" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1279" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1279">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1280" spans="1:8">
-      <c r="A1280" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1280">
-        <v>81</v>
-      </c>
-      <c r="C1280">
-        <v>56</v>
-      </c>
-      <c r="D1280" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1280" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1280" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1280" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1280">
-        <v>3</v>
-      </c>
+    <row r="1261" spans="1:7">
+      <c r="A1261" s="1"/>
+    </row>
+    <row r="1262" spans="1:7">
+      <c r="A1262" s="1"/>
+    </row>
+    <row r="1263" spans="1:7">
+      <c r="A1263" s="1"/>
+    </row>
+    <row r="1265" spans="1:1">
+      <c r="A1265" s="1"/>
+    </row>
+    <row r="1266" spans="1:1">
+      <c r="A1266" s="1"/>
+    </row>
+    <row r="1267" spans="1:1">
+      <c r="A1267" s="1"/>
+    </row>
+    <row r="1268" spans="1:1">
+      <c r="A1268" s="1"/>
+    </row>
+    <row r="1269" spans="1:1">
+      <c r="A1269" s="1"/>
+    </row>
+    <row r="1270" spans="1:1">
+      <c r="A1270" s="1"/>
+    </row>
+    <row r="1271" spans="1:1">
+      <c r="A1271" s="1"/>
+    </row>
+    <row r="1272" spans="1:1">
+      <c r="A1272" s="1"/>
+    </row>
+    <row r="1273" spans="1:1">
+      <c r="A1273" s="1"/>
+    </row>
+    <row r="1274" spans="1:1">
+      <c r="A1274" s="1"/>
+    </row>
+    <row r="1275" spans="1:1">
+      <c r="A1275" s="1"/>
+    </row>
+    <row r="1276" spans="1:1">
+      <c r="A1276" s="1"/>
+    </row>
+    <row r="1277" spans="1:1">
+      <c r="A1277" s="1"/>
+    </row>
+    <row r="1278" spans="1:1">
+      <c r="A1278" s="1"/>
+    </row>
+    <row r="1279" spans="1:1">
+      <c r="A1279" s="1"/>
+    </row>
+    <row r="1280" spans="1:1">
+      <c r="A1280" s="1"/>
     </row>
     <row r="1281" spans="1:8">
-      <c r="A1281" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1281">
-        <v>80</v>
-      </c>
-      <c r="C1281">
-        <v>56</v>
-      </c>
-      <c r="D1281" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1281" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1281" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1281" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1281">
-        <v>3</v>
-      </c>
+      <c r="A1281" s="1"/>
     </row>
     <row r="1282" spans="1:8">
       <c r="A1282" s="1">
@@ -30107,7 +29643,7 @@
         <v>5023</v>
       </c>
       <c r="B1408">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C1408">
         <v>56</v>
@@ -30122,531 +29658,72 @@
         <v>2</v>
       </c>
       <c r="G1408" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1408">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1409" spans="1:8">
-      <c r="A1409" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1409">
-        <v>74</v>
-      </c>
-      <c r="C1409">
-        <v>56</v>
-      </c>
-      <c r="D1409" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1409" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1409" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1409" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1409">
-        <v>2</v>
-      </c>
+      <c r="A1409" s="1"/>
+      <c r="H1409" s="3"/>
     </row>
     <row r="1410" spans="1:8">
-      <c r="A1410" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1410">
-        <v>68</v>
-      </c>
-      <c r="C1410">
-        <v>44</v>
-      </c>
-      <c r="D1410" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1410" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1410" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1410" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1410">
-        <v>3</v>
-      </c>
+      <c r="A1410" s="1"/>
     </row>
     <row r="1411" spans="1:8">
-      <c r="A1411" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1411">
-        <v>76</v>
-      </c>
-      <c r="C1411">
-        <v>56</v>
-      </c>
-      <c r="D1411" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1411" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1411" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1411" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1411">
-        <v>3</v>
-      </c>
+      <c r="A1411" s="1"/>
     </row>
     <row r="1412" spans="1:8">
-      <c r="A1412" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1412">
-        <v>74</v>
-      </c>
-      <c r="C1412">
-        <v>56</v>
-      </c>
-      <c r="D1412" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1412" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1412" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1412" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1412">
-        <v>2</v>
-      </c>
+      <c r="A1412" s="1"/>
     </row>
     <row r="1413" spans="1:8">
-      <c r="A1413" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1413">
-        <v>68</v>
-      </c>
-      <c r="C1413">
-        <v>56</v>
-      </c>
-      <c r="D1413" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1413" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1413" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1413" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1413">
-        <v>3</v>
-      </c>
+      <c r="A1413" s="1"/>
     </row>
     <row r="1414" spans="1:8">
-      <c r="A1414" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1414">
-        <v>76</v>
-      </c>
-      <c r="C1414">
-        <v>56</v>
-      </c>
-      <c r="D1414" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1414" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1414" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1414" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1414">
-        <v>3</v>
-      </c>
+      <c r="A1414" s="1"/>
     </row>
     <row r="1415" spans="1:8">
-      <c r="A1415" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1415">
-        <v>73</v>
-      </c>
-      <c r="C1415">
-        <v>56</v>
-      </c>
-      <c r="D1415" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1415" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1415" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1415" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1415">
-        <v>2</v>
-      </c>
+      <c r="A1415" s="1"/>
     </row>
     <row r="1416" spans="1:8">
-      <c r="A1416" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1416">
-        <v>73</v>
-      </c>
-      <c r="C1416">
-        <v>56</v>
-      </c>
-      <c r="D1416" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1416" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1416" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1416" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1416">
-        <v>3</v>
-      </c>
+      <c r="A1416" s="1"/>
     </row>
     <row r="1417" spans="1:8">
-      <c r="A1417" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1417">
-        <v>77</v>
-      </c>
-      <c r="C1417">
-        <v>56</v>
-      </c>
-      <c r="D1417" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1417" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1417" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1417" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1417">
-        <v>3</v>
-      </c>
+      <c r="A1417" s="1"/>
     </row>
     <row r="1418" spans="1:8">
-      <c r="A1418" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1418">
-        <v>73</v>
-      </c>
-      <c r="C1418">
-        <v>56</v>
-      </c>
-      <c r="D1418" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1418" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1418" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1418" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1418">
-        <v>3</v>
-      </c>
+      <c r="A1418" s="1"/>
     </row>
     <row r="1419" spans="1:8">
-      <c r="A1419" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1419">
-        <v>74</v>
-      </c>
-      <c r="C1419">
-        <v>56</v>
-      </c>
-      <c r="D1419" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1419" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1419" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1419" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1419">
-        <v>3</v>
-      </c>
+      <c r="A1419" s="1"/>
     </row>
     <row r="1420" spans="1:8">
-      <c r="A1420" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1420">
-        <v>76</v>
-      </c>
-      <c r="C1420">
-        <v>56</v>
-      </c>
-      <c r="D1420" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1420" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1420" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1420" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1420">
-        <v>3</v>
-      </c>
+      <c r="A1420" s="1"/>
     </row>
     <row r="1421" spans="1:8">
-      <c r="A1421" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1421">
-        <v>73</v>
-      </c>
-      <c r="C1421">
-        <v>56</v>
-      </c>
-      <c r="D1421" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1421" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1421" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1421" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1421">
-        <v>2</v>
-      </c>
+      <c r="A1421" s="1"/>
     </row>
     <row r="1422" spans="1:8">
-      <c r="A1422" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1422">
-        <v>73</v>
-      </c>
-      <c r="C1422">
-        <v>56</v>
-      </c>
-      <c r="D1422" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1422" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1422" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1422" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1422">
-        <v>3</v>
-      </c>
+      <c r="A1422" s="1"/>
     </row>
     <row r="1423" spans="1:8">
-      <c r="A1423" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1423">
-        <v>74</v>
-      </c>
-      <c r="C1423">
-        <v>56</v>
-      </c>
-      <c r="D1423" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1423" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1423" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1423" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1423">
-        <v>3</v>
-      </c>
+      <c r="A1423" s="1"/>
     </row>
     <row r="1424" spans="1:8">
-      <c r="A1424" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1424">
-        <v>76</v>
-      </c>
-      <c r="C1424">
-        <v>56</v>
-      </c>
-      <c r="D1424" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1424" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1424" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1424" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1424">
-        <v>3</v>
-      </c>
+      <c r="A1424" s="1"/>
     </row>
     <row r="1425" spans="1:8">
-      <c r="A1425" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1425">
-        <v>69</v>
-      </c>
-      <c r="C1425">
-        <v>56</v>
-      </c>
-      <c r="D1425" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1425" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1425" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1425" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1425">
-        <v>3</v>
-      </c>
+      <c r="A1425" s="1"/>
     </row>
     <row r="1426" spans="1:8">
-      <c r="A1426" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1426">
-        <v>76</v>
-      </c>
-      <c r="C1426">
-        <v>56</v>
-      </c>
-      <c r="D1426" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1426" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1426" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1426" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1426">
-        <v>3</v>
-      </c>
+      <c r="A1426" s="1"/>
     </row>
     <row r="1427" spans="1:8">
-      <c r="A1427" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1427">
-        <v>77</v>
-      </c>
-      <c r="C1427">
-        <v>56</v>
-      </c>
-      <c r="D1427" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1427" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1427" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1427" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1427">
-        <v>3</v>
-      </c>
+      <c r="A1427" s="1"/>
     </row>
     <row r="1428" spans="1:8">
-      <c r="A1428" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1428">
-        <v>73</v>
-      </c>
-      <c r="C1428">
-        <v>56</v>
-      </c>
-      <c r="D1428" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1428" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1428" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1428" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1428">
-        <v>3</v>
-      </c>
+      <c r="A1428" s="1"/>
     </row>
     <row r="1429" spans="1:8">
       <c r="A1429" s="1">
@@ -31673,84 +30750,44 @@
       </c>
     </row>
     <row r="1473" spans="1:8">
-      <c r="A1473" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1473">
-        <v>69</v>
-      </c>
-      <c r="C1473">
-        <v>44</v>
-      </c>
-      <c r="D1473" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1473" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1473" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1473" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1473">
-        <v>3</v>
-      </c>
+      <c r="A1473" s="2"/>
+      <c r="B1473" s="3"/>
+      <c r="C1473" s="3"/>
+      <c r="D1473" s="3"/>
+      <c r="E1473" s="3"/>
+      <c r="F1473" s="3"/>
+      <c r="G1473" s="3"/>
+      <c r="H1473" s="3"/>
     </row>
     <row r="1474" spans="1:8">
-      <c r="D1474" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1474" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1474" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1474" t="s">
-        <v>3</v>
-      </c>
+      <c r="A1474" s="3"/>
+      <c r="B1474" s="3"/>
+      <c r="C1474" s="3"/>
+      <c r="D1474" s="3"/>
+      <c r="E1474" s="3"/>
+      <c r="F1474" s="3"/>
+      <c r="G1474" s="3"/>
+      <c r="H1474" s="3"/>
     </row>
     <row r="1475" spans="1:8">
-      <c r="D1475" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1475" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1475" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1475" t="s">
-        <v>4</v>
-      </c>
+      <c r="A1475" s="3"/>
+      <c r="B1475" s="3"/>
+      <c r="C1475" s="3"/>
+      <c r="D1475" s="3"/>
+      <c r="E1475" s="3"/>
+      <c r="F1475" s="3"/>
+      <c r="G1475" s="3"/>
+      <c r="H1475" s="3"/>
     </row>
     <row r="1476" spans="1:8">
-      <c r="A1476" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1476">
-        <v>69</v>
-      </c>
-      <c r="C1476">
-        <v>56</v>
-      </c>
-      <c r="D1476" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1476" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1476" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1476" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1476">
-        <v>3</v>
-      </c>
+      <c r="A1476" s="2"/>
+      <c r="B1476" s="3"/>
+      <c r="C1476" s="3"/>
+      <c r="D1476" s="3"/>
+      <c r="E1476" s="3"/>
+      <c r="F1476" s="3"/>
+      <c r="G1476" s="3"/>
+      <c r="H1476" s="3"/>
     </row>
     <row r="1477" spans="1:8">
       <c r="D1477" t="s">
@@ -31781,30 +30818,7 @@
       </c>
     </row>
     <row r="1479" spans="1:8">
-      <c r="A1479" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1479">
-        <v>73</v>
-      </c>
-      <c r="C1479">
-        <v>56</v>
-      </c>
-      <c r="D1479" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1479" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1479" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1479" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1479">
-        <v>3</v>
-      </c>
+      <c r="A1479" s="1"/>
     </row>
     <row r="1480" spans="1:8">
       <c r="D1480" t="s">
@@ -33943,538 +32957,64 @@
       </c>
     </row>
     <row r="1576" spans="1:8">
-      <c r="A1576" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1576">
-        <v>82</v>
-      </c>
-      <c r="C1576">
-        <v>56</v>
-      </c>
-      <c r="D1576" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1576" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1576" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1576" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1576">
-        <v>3</v>
-      </c>
+      <c r="A1576" s="1"/>
     </row>
     <row r="1577" spans="1:8">
-      <c r="A1577" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1577">
-        <v>83</v>
-      </c>
-      <c r="C1577">
-        <v>56</v>
-      </c>
-      <c r="D1577" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1577" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1577" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1577" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1577">
-        <v>3</v>
-      </c>
+      <c r="A1577" s="1"/>
     </row>
     <row r="1578" spans="1:8">
-      <c r="A1578" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1578">
-        <v>81</v>
-      </c>
-      <c r="C1578">
-        <v>56</v>
-      </c>
-      <c r="D1578" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1578" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1578" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1578" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1578">
-        <v>3</v>
-      </c>
+      <c r="A1578" s="1"/>
     </row>
     <row r="1579" spans="1:8">
-      <c r="A1579" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1579">
-        <v>83</v>
-      </c>
-      <c r="C1579">
-        <v>56</v>
-      </c>
-      <c r="D1579" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1579" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1579" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1579" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1579">
-        <v>3</v>
-      </c>
+      <c r="A1579" s="1"/>
     </row>
     <row r="1580" spans="1:8">
-      <c r="A1580" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1580">
-        <v>82</v>
-      </c>
-      <c r="C1580">
-        <v>56</v>
-      </c>
-      <c r="D1580" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1580" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1580" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1580" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1580">
-        <v>3</v>
-      </c>
+      <c r="A1580" s="1"/>
     </row>
     <row r="1581" spans="1:8">
-      <c r="A1581" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1581">
-        <v>82</v>
-      </c>
-      <c r="C1581">
-        <v>56</v>
-      </c>
-      <c r="D1581" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1581" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1581" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1581" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1581">
-        <v>3</v>
-      </c>
+      <c r="A1581" s="1"/>
     </row>
     <row r="1582" spans="1:8">
-      <c r="A1582" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1582">
-        <v>84</v>
-      </c>
-      <c r="C1582">
-        <v>56</v>
-      </c>
-      <c r="D1582" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1582" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1582" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1582" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1582">
-        <v>3</v>
-      </c>
+      <c r="A1582" s="1"/>
     </row>
     <row r="1583" spans="1:8">
-      <c r="A1583" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1583">
-        <v>83</v>
-      </c>
-      <c r="C1583">
-        <v>56</v>
-      </c>
-      <c r="D1583" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1583" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1583" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1583" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1583">
-        <v>3</v>
-      </c>
+      <c r="A1583" s="1"/>
     </row>
     <row r="1584" spans="1:8">
-      <c r="A1584" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1584">
-        <v>82</v>
-      </c>
-      <c r="C1584">
-        <v>56</v>
-      </c>
-      <c r="D1584" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1584" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1584" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1584" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1584">
-        <v>3</v>
-      </c>
+      <c r="A1584" s="1"/>
     </row>
     <row r="1585" spans="1:8">
-      <c r="A1585" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1585">
-        <v>84</v>
-      </c>
-      <c r="C1585">
-        <v>56</v>
-      </c>
-      <c r="D1585" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1585" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1585" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1585" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1585">
-        <v>3</v>
-      </c>
+      <c r="A1585" s="1"/>
     </row>
     <row r="1586" spans="1:8">
-      <c r="A1586" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1586">
-        <v>82</v>
-      </c>
-      <c r="C1586">
-        <v>56</v>
-      </c>
-      <c r="D1586" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1586" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1586" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1586" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1586">
-        <v>3</v>
-      </c>
+      <c r="A1586" s="1"/>
     </row>
     <row r="1587" spans="1:8">
-      <c r="A1587" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1587">
-        <v>82</v>
-      </c>
-      <c r="C1587">
-        <v>56</v>
-      </c>
-      <c r="D1587" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1587" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1587" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1587" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1587">
-        <v>3</v>
-      </c>
+      <c r="A1587" s="1"/>
     </row>
     <row r="1588" spans="1:8">
-      <c r="A1588" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1588">
-        <v>84</v>
-      </c>
-      <c r="C1588">
-        <v>56</v>
-      </c>
-      <c r="D1588" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1588" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1588" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1588" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1588">
-        <v>3</v>
-      </c>
+      <c r="A1588" s="1"/>
     </row>
     <row r="1589" spans="1:8">
-      <c r="A1589" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1589">
-        <v>83</v>
-      </c>
-      <c r="C1589">
-        <v>56</v>
-      </c>
-      <c r="D1589" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1589" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1589" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1589" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1589">
-        <v>3</v>
-      </c>
+      <c r="A1589" s="1"/>
     </row>
     <row r="1590" spans="1:8">
-      <c r="A1590" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1590">
-        <v>82</v>
-      </c>
-      <c r="C1590">
-        <v>56</v>
-      </c>
-      <c r="D1590" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1590" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1590" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1590" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1590">
-        <v>3</v>
-      </c>
+      <c r="A1590" s="1"/>
     </row>
     <row r="1591" spans="1:8">
-      <c r="A1591" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1591">
-        <v>84</v>
-      </c>
-      <c r="C1591">
-        <v>56</v>
-      </c>
-      <c r="D1591" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1591" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1591" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1591" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1591">
-        <v>3</v>
-      </c>
+      <c r="A1591" s="1"/>
     </row>
     <row r="1592" spans="1:8">
-      <c r="A1592" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1592">
-        <v>84</v>
-      </c>
-      <c r="C1592">
-        <v>56</v>
-      </c>
-      <c r="D1592" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1592" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1592" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1592" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1592">
-        <v>3</v>
-      </c>
+      <c r="A1592" s="1"/>
     </row>
     <row r="1593" spans="1:8">
-      <c r="A1593" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1593">
-        <v>83</v>
-      </c>
-      <c r="C1593">
-        <v>56</v>
-      </c>
-      <c r="D1593" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1593" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1593" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1593" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1593">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1594" spans="1:8">
-      <c r="D1594" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1594" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1594" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1594" t="s">
-        <v>3</v>
-      </c>
+      <c r="A1593" s="1"/>
     </row>
     <row r="1595" spans="1:8">
-      <c r="A1595" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1595">
-        <v>84</v>
-      </c>
-      <c r="C1595">
-        <v>56</v>
-      </c>
-      <c r="D1595" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1595" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1595" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1595" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1595">
-        <v>3</v>
-      </c>
+      <c r="A1595" s="1"/>
     </row>
     <row r="1596" spans="1:8">
-      <c r="A1596" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1596">
-        <v>83</v>
-      </c>
-      <c r="C1596">
-        <v>56</v>
-      </c>
-      <c r="D1596" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1596" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1596" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1596" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1596">
-        <v>3</v>
-      </c>
+      <c r="A1596" s="1"/>
     </row>
     <row r="1597" spans="1:8">
       <c r="A1597" s="1">
@@ -38640,7 +37180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1825" spans="1:8">
+    <row r="1825" spans="1:7">
       <c r="D1825" t="s">
         <v>34</v>
       </c>
@@ -38654,7 +37194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1826" spans="1:8">
+    <row r="1826" spans="1:7">
       <c r="D1826" t="s">
         <v>34</v>
       </c>
@@ -38668,7 +37208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1827" spans="1:8">
+    <row r="1827" spans="1:7">
       <c r="D1827" t="s">
         <v>34</v>
       </c>
@@ -38682,7 +37222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1828" spans="1:8">
+    <row r="1828" spans="1:7">
       <c r="D1828" t="s">
         <v>34</v>
       </c>
@@ -38696,7 +37236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1829" spans="1:8">
+    <row r="1829" spans="1:7">
       <c r="D1829" t="s">
         <v>34</v>
       </c>
@@ -38710,877 +37250,83 @@
         <v>4</v>
       </c>
     </row>
-    <row r="1830" spans="1:8">
-      <c r="A1830" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1830">
-        <v>89</v>
-      </c>
-      <c r="C1830">
-        <v>56</v>
-      </c>
-      <c r="D1830" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1830" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1830" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1830" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1830">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1831" spans="1:8">
-      <c r="D1831" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1831" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1831" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1831" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1832" spans="1:8">
-      <c r="D1832" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1832" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1832" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1832" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1833" spans="1:8">
-      <c r="A1833" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1833">
-        <v>88</v>
-      </c>
-      <c r="C1833">
-        <v>56</v>
-      </c>
-      <c r="D1833" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1833" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1833" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1833" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1833">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1834" spans="1:8">
-      <c r="D1834" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1834" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1834" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1834" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1835" spans="1:8">
-      <c r="D1835" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1835" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1835" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1835" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1836" spans="1:8">
-      <c r="A1836" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1836">
-        <v>90</v>
-      </c>
-      <c r="C1836">
-        <v>56</v>
-      </c>
-      <c r="D1836" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1836" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1836" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1836" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1836">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1837" spans="1:8">
-      <c r="D1837" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1837" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1837" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1837" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1838" spans="1:8">
-      <c r="D1838" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1838" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1838" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1838" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1839" spans="1:8">
-      <c r="A1839" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1839">
-        <v>90</v>
-      </c>
-      <c r="C1839">
-        <v>56</v>
-      </c>
-      <c r="D1839" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1839" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1839" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1839" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1839">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1840" spans="1:8">
-      <c r="D1840" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1840" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1840" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1840" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1841" spans="1:8">
-      <c r="D1841" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1841" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1841" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1841" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1842" spans="1:8">
-      <c r="A1842" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1842">
-        <v>90</v>
-      </c>
-      <c r="C1842">
-        <v>56</v>
-      </c>
-      <c r="D1842" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1842" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1842" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1842" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1842">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1843" spans="1:8">
-      <c r="D1843" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1843" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1843" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1843" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1844" spans="1:8">
-      <c r="D1844" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1844" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1844" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1844" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1845" spans="1:8">
-      <c r="D1845" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1845" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1845" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1845" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="1846" spans="1:8">
-      <c r="D1846" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1846" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1846" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1846" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1847" spans="1:8">
-      <c r="D1847" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1847" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1847" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1847" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1848" spans="1:8">
-      <c r="D1848" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1848" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1848" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1848" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="1849" spans="1:8">
-      <c r="A1849" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1849">
-        <v>88</v>
-      </c>
-      <c r="C1849">
-        <v>56</v>
-      </c>
-      <c r="D1849" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1849" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1849" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1849" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1849">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1850" spans="1:8">
-      <c r="A1850" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1850">
-        <v>87</v>
-      </c>
-      <c r="C1850">
-        <v>56</v>
-      </c>
-      <c r="D1850" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1850" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1850" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1850" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1850">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1851" spans="1:8">
-      <c r="A1851" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1851">
-        <v>87</v>
-      </c>
-      <c r="C1851">
-        <v>56</v>
-      </c>
-      <c r="D1851" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1851" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1851" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1851" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1851">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1852" spans="1:8">
-      <c r="A1852" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1852">
-        <v>81</v>
-      </c>
-      <c r="C1852">
-        <v>15</v>
-      </c>
-      <c r="D1852" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1852" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1852" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1852" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1852">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1853" spans="1:8">
-      <c r="A1853" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1853">
-        <v>87</v>
-      </c>
-      <c r="C1853">
-        <v>56</v>
-      </c>
-      <c r="D1853" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1853" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1853" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1853" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1853">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1854" spans="1:8">
-      <c r="A1854" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1854">
-        <v>87</v>
-      </c>
-      <c r="C1854">
-        <v>56</v>
-      </c>
-      <c r="D1854" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1854" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1854" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1854" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1854">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1855" spans="1:8">
-      <c r="A1855" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1855">
-        <v>89</v>
-      </c>
-      <c r="C1855">
-        <v>56</v>
-      </c>
-      <c r="D1855" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1855" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1855" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1855" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1855">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1856" spans="1:8">
-      <c r="A1856" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1856">
-        <v>88</v>
-      </c>
-      <c r="C1856">
-        <v>56</v>
-      </c>
-      <c r="D1856" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1856" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1856" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1856" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1856">
-        <v>3</v>
-      </c>
+    <row r="1830" spans="1:7">
+      <c r="A1830" s="1"/>
+    </row>
+    <row r="1833" spans="1:7">
+      <c r="A1833" s="1"/>
+    </row>
+    <row r="1836" spans="1:7">
+      <c r="A1836" s="1"/>
+    </row>
+    <row r="1839" spans="1:7">
+      <c r="A1839" s="1"/>
+    </row>
+    <row r="1842" spans="1:1">
+      <c r="A1842" s="1"/>
+    </row>
+    <row r="1849" spans="1:1">
+      <c r="A1849" s="1"/>
+    </row>
+    <row r="1850" spans="1:1">
+      <c r="A1850" s="1"/>
+    </row>
+    <row r="1851" spans="1:1">
+      <c r="A1851" s="1"/>
+    </row>
+    <row r="1852" spans="1:1">
+      <c r="A1852" s="1"/>
+    </row>
+    <row r="1853" spans="1:1">
+      <c r="A1853" s="1"/>
+    </row>
+    <row r="1854" spans="1:1">
+      <c r="A1854" s="1"/>
+    </row>
+    <row r="1855" spans="1:1">
+      <c r="A1855" s="1"/>
+    </row>
+    <row r="1856" spans="1:1">
+      <c r="A1856" s="1"/>
     </row>
     <row r="1857" spans="1:8">
-      <c r="A1857" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1857">
-        <v>87</v>
-      </c>
-      <c r="C1857">
-        <v>56</v>
-      </c>
-      <c r="D1857" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1857" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1857" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1857" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1857">
-        <v>3</v>
-      </c>
+      <c r="A1857" s="1"/>
     </row>
     <row r="1858" spans="1:8">
-      <c r="A1858" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1858">
-        <v>89</v>
-      </c>
-      <c r="C1858">
-        <v>56</v>
-      </c>
-      <c r="D1858" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1858" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1858" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1858" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1858">
-        <v>3</v>
-      </c>
+      <c r="A1858" s="1"/>
     </row>
     <row r="1859" spans="1:8">
-      <c r="A1859" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1859">
-        <v>88</v>
-      </c>
-      <c r="C1859">
-        <v>56</v>
-      </c>
-      <c r="D1859" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1859" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1859" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1859" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1859">
-        <v>3</v>
-      </c>
+      <c r="A1859" s="1"/>
     </row>
     <row r="1860" spans="1:8">
-      <c r="A1860" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1860">
-        <v>87</v>
-      </c>
-      <c r="C1860">
-        <v>56</v>
-      </c>
-      <c r="D1860" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1860" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1860" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1860" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1860">
-        <v>3</v>
-      </c>
+      <c r="A1860" s="1"/>
     </row>
     <row r="1861" spans="1:8">
-      <c r="A1861" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1861">
-        <v>88</v>
-      </c>
-      <c r="C1861">
-        <v>56</v>
-      </c>
-      <c r="D1861" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1861" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1861" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1861" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1861">
-        <v>3</v>
-      </c>
+      <c r="A1861" s="1"/>
     </row>
     <row r="1862" spans="1:8">
-      <c r="A1862" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1862">
-        <v>88</v>
-      </c>
-      <c r="C1862">
-        <v>56</v>
-      </c>
-      <c r="D1862" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1862" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1862" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1862" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1862">
-        <v>3</v>
-      </c>
+      <c r="A1862" s="1"/>
     </row>
     <row r="1863" spans="1:8">
-      <c r="A1863" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1863">
-        <v>87</v>
-      </c>
-      <c r="C1863">
-        <v>56</v>
-      </c>
-      <c r="D1863" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1863" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1863" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1863" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1863">
-        <v>3</v>
-      </c>
+      <c r="A1863" s="1"/>
     </row>
     <row r="1864" spans="1:8">
-      <c r="A1864" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1864">
-        <v>89</v>
-      </c>
-      <c r="C1864">
-        <v>56</v>
-      </c>
-      <c r="D1864" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1864" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1864" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1864" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1864">
-        <v>3</v>
-      </c>
+      <c r="A1864" s="1"/>
     </row>
     <row r="1865" spans="1:8">
-      <c r="A1865" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1865">
-        <v>88</v>
-      </c>
-      <c r="C1865">
-        <v>56</v>
-      </c>
-      <c r="D1865" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1865" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1865" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1865" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1865">
-        <v>3</v>
-      </c>
+      <c r="A1865" s="1"/>
     </row>
     <row r="1866" spans="1:8">
-      <c r="A1866" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1866">
-        <v>84</v>
-      </c>
-      <c r="C1866">
-        <v>56</v>
-      </c>
-      <c r="D1866" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1866" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1866" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1866" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1866">
-        <v>3</v>
-      </c>
+      <c r="A1866" s="1"/>
     </row>
     <row r="1867" spans="1:8">
-      <c r="A1867" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1867">
-        <v>89</v>
-      </c>
-      <c r="C1867">
-        <v>56</v>
-      </c>
-      <c r="D1867" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1867" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1867" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1867" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1867">
-        <v>3</v>
-      </c>
+      <c r="A1867" s="1"/>
     </row>
     <row r="1868" spans="1:8">
-      <c r="A1868" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1868">
-        <v>88</v>
-      </c>
-      <c r="C1868">
-        <v>56</v>
-      </c>
-      <c r="D1868" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1868" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1868" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1868" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1868">
-        <v>3</v>
-      </c>
+      <c r="A1868" s="1"/>
     </row>
     <row r="1869" spans="1:8">
-      <c r="A1869" s="1">
-        <v>5023</v>
-      </c>
-      <c r="B1869">
-        <v>87</v>
-      </c>
-      <c r="C1869">
-        <v>56</v>
-      </c>
-      <c r="D1869" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1869" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1869" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1869" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1869">
-        <v>3</v>
-      </c>
+      <c r="A1869" s="1"/>
     </row>
     <row r="1870" spans="1:8">
       <c r="A1870" s="1">
@@ -42194,5 +39940,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>